<commit_message>
final changes updating readme and ppt
</commit_message>
<xml_diff>
--- a/doc/RegisterMapping.xlsx
+++ b/doc/RegisterMapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/varunposimsetty/Desktop/SAL_TaskAssignment/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB11A0A5-69C8-594D-BDC9-34BCA5EC6E3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB002D97-203E-C645-973C-254ABC55AE1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" xr2:uid="{DE537055-B1E9-4F17-92F2-EA73B7270BD6}"/>
   </bookViews>
@@ -89,9 +89,6 @@
     <t>Result (Sign Extended)</t>
   </si>
   <si>
-    <t>w</t>
-  </si>
-  <si>
     <t>status</t>
   </si>
   <si>
@@ -99,6 +96,9 @@
   </si>
   <si>
     <t>pipe_status</t>
+  </si>
+  <si>
+    <t>w+r</t>
   </si>
 </sst>
 </file>
@@ -316,24 +316,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -346,15 +328,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -363,6 +336,33 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -704,7 +704,7 @@
   <dimension ref="A4:AL14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="66" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:AK12"/>
+      <selection activeCell="Q21" sqref="Q21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -715,92 +715,92 @@
   <sheetData>
     <row r="4" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="3" t="s">
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="4"/>
-      <c r="O4" s="4"/>
-      <c r="P4" s="4"/>
-      <c r="Q4" s="4"/>
-      <c r="R4" s="4"/>
-      <c r="S4" s="4"/>
-      <c r="T4" s="4"/>
-      <c r="U4" s="4"/>
-      <c r="V4" s="4"/>
-      <c r="W4" s="4"/>
-      <c r="X4" s="4"/>
-      <c r="Y4" s="4"/>
-      <c r="Z4" s="4"/>
-      <c r="AA4" s="4"/>
-      <c r="AB4" s="4"/>
-      <c r="AC4" s="4"/>
-      <c r="AD4" s="4"/>
-      <c r="AE4" s="4"/>
-      <c r="AF4" s="4"/>
-      <c r="AG4" s="4"/>
-      <c r="AH4" s="4"/>
-      <c r="AI4" s="4"/>
-      <c r="AJ4" s="4"/>
-      <c r="AK4" s="5"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="14"/>
+      <c r="N4" s="14"/>
+      <c r="O4" s="14"/>
+      <c r="P4" s="14"/>
+      <c r="Q4" s="14"/>
+      <c r="R4" s="14"/>
+      <c r="S4" s="14"/>
+      <c r="T4" s="14"/>
+      <c r="U4" s="14"/>
+      <c r="V4" s="14"/>
+      <c r="W4" s="14"/>
+      <c r="X4" s="14"/>
+      <c r="Y4" s="14"/>
+      <c r="Z4" s="14"/>
+      <c r="AA4" s="14"/>
+      <c r="AB4" s="14"/>
+      <c r="AC4" s="14"/>
+      <c r="AD4" s="14"/>
+      <c r="AE4" s="14"/>
+      <c r="AF4" s="14"/>
+      <c r="AG4" s="14"/>
+      <c r="AH4" s="14"/>
+      <c r="AI4" s="14"/>
+      <c r="AJ4" s="14"/>
+      <c r="AK4" s="15"/>
       <c r="AL4" s="1"/>
     </row>
     <row r="5" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
-      <c r="L5" s="7"/>
-      <c r="M5" s="7"/>
-      <c r="N5" s="7"/>
-      <c r="O5" s="7"/>
-      <c r="P5" s="7"/>
-      <c r="Q5" s="7"/>
-      <c r="R5" s="7"/>
-      <c r="S5" s="7"/>
-      <c r="T5" s="7"/>
-      <c r="U5" s="7"/>
-      <c r="V5" s="7"/>
-      <c r="W5" s="7"/>
-      <c r="X5" s="7"/>
-      <c r="Y5" s="7"/>
-      <c r="Z5" s="7"/>
-      <c r="AA5" s="7"/>
-      <c r="AB5" s="7"/>
-      <c r="AC5" s="7"/>
-      <c r="AD5" s="7"/>
-      <c r="AE5" s="7"/>
-      <c r="AF5" s="7"/>
-      <c r="AG5" s="7"/>
-      <c r="AH5" s="7"/>
-      <c r="AI5" s="7"/>
-      <c r="AJ5" s="7"/>
-      <c r="AK5" s="8"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="17"/>
+      <c r="K5" s="17"/>
+      <c r="L5" s="17"/>
+      <c r="M5" s="17"/>
+      <c r="N5" s="17"/>
+      <c r="O5" s="17"/>
+      <c r="P5" s="17"/>
+      <c r="Q5" s="17"/>
+      <c r="R5" s="17"/>
+      <c r="S5" s="17"/>
+      <c r="T5" s="17"/>
+      <c r="U5" s="17"/>
+      <c r="V5" s="17"/>
+      <c r="W5" s="17"/>
+      <c r="X5" s="17"/>
+      <c r="Y5" s="17"/>
+      <c r="Z5" s="17"/>
+      <c r="AA5" s="17"/>
+      <c r="AB5" s="17"/>
+      <c r="AC5" s="17"/>
+      <c r="AD5" s="17"/>
+      <c r="AE5" s="17"/>
+      <c r="AF5" s="17"/>
+      <c r="AG5" s="17"/>
+      <c r="AH5" s="17"/>
+      <c r="AI5" s="17"/>
+      <c r="AJ5" s="17"/>
+      <c r="AK5" s="18"/>
       <c r="AL5" s="1"/>
     </row>
     <row r="6" spans="1:38" ht="23" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="10"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="4"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
@@ -837,350 +837,350 @@
     </row>
     <row r="7" spans="1:38" ht="24" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="12"/>
-      <c r="D7" s="11" t="s">
+      <c r="C7" s="6"/>
+      <c r="D7" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E7" s="10"/>
-      <c r="F7" s="11">
+      <c r="E7" s="4"/>
+      <c r="F7" s="5">
         <v>31</v>
       </c>
-      <c r="G7" s="11">
+      <c r="G7" s="5">
         <v>30</v>
       </c>
-      <c r="H7" s="11">
+      <c r="H7" s="5">
         <v>29</v>
       </c>
-      <c r="I7" s="11">
+      <c r="I7" s="5">
         <v>28</v>
       </c>
-      <c r="J7" s="11">
+      <c r="J7" s="5">
         <v>27</v>
       </c>
-      <c r="K7" s="11">
+      <c r="K7" s="5">
         <v>26</v>
       </c>
-      <c r="L7" s="11">
+      <c r="L7" s="5">
         <v>25</v>
       </c>
-      <c r="M7" s="11">
+      <c r="M7" s="5">
         <v>24</v>
       </c>
-      <c r="N7" s="11">
+      <c r="N7" s="5">
         <v>23</v>
       </c>
-      <c r="O7" s="11">
+      <c r="O7" s="5">
         <v>22</v>
       </c>
-      <c r="P7" s="11">
+      <c r="P7" s="5">
         <v>21</v>
       </c>
-      <c r="Q7" s="11">
+      <c r="Q7" s="5">
         <v>20</v>
       </c>
-      <c r="R7" s="11">
+      <c r="R7" s="5">
         <v>19</v>
       </c>
-      <c r="S7" s="11">
+      <c r="S7" s="5">
         <v>18</v>
       </c>
-      <c r="T7" s="11">
+      <c r="T7" s="5">
         <v>17</v>
       </c>
-      <c r="U7" s="11">
+      <c r="U7" s="5">
         <v>16</v>
       </c>
-      <c r="V7" s="11">
+      <c r="V7" s="5">
         <v>15</v>
       </c>
-      <c r="W7" s="11">
+      <c r="W7" s="5">
         <v>14</v>
       </c>
-      <c r="X7" s="11">
+      <c r="X7" s="5">
         <v>13</v>
       </c>
-      <c r="Y7" s="11">
+      <c r="Y7" s="5">
         <v>12</v>
       </c>
-      <c r="Z7" s="11">
+      <c r="Z7" s="5">
         <v>11</v>
       </c>
-      <c r="AA7" s="11">
+      <c r="AA7" s="5">
         <v>10</v>
       </c>
-      <c r="AB7" s="11">
+      <c r="AB7" s="5">
         <v>9</v>
       </c>
-      <c r="AC7" s="11">
+      <c r="AC7" s="5">
         <v>8</v>
       </c>
-      <c r="AD7" s="11">
+      <c r="AD7" s="5">
         <v>7</v>
       </c>
-      <c r="AE7" s="11">
+      <c r="AE7" s="5">
         <v>6</v>
       </c>
-      <c r="AF7" s="11">
+      <c r="AF7" s="5">
         <v>5</v>
       </c>
-      <c r="AG7" s="11">
+      <c r="AG7" s="5">
         <v>4</v>
       </c>
-      <c r="AH7" s="11">
+      <c r="AH7" s="5">
         <v>3</v>
       </c>
-      <c r="AI7" s="11">
+      <c r="AI7" s="5">
         <v>2</v>
       </c>
-      <c r="AJ7" s="11">
+      <c r="AJ7" s="5">
         <v>1</v>
       </c>
-      <c r="AK7" s="11">
+      <c r="AK7" s="5">
         <v>0</v>
       </c>
       <c r="AL7" s="1"/>
     </row>
     <row r="8" spans="1:38" ht="23" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="9"/>
-      <c r="L8" s="9"/>
-      <c r="M8" s="9"/>
-      <c r="N8" s="9"/>
-      <c r="O8" s="9"/>
-      <c r="P8" s="9"/>
-      <c r="Q8" s="9"/>
-      <c r="R8" s="9"/>
-      <c r="S8" s="9"/>
-      <c r="T8" s="9"/>
-      <c r="U8" s="9"/>
-      <c r="V8" s="9"/>
-      <c r="W8" s="9"/>
-      <c r="X8" s="9"/>
-      <c r="Y8" s="9"/>
-      <c r="Z8" s="9"/>
-      <c r="AA8" s="9"/>
-      <c r="AB8" s="9"/>
-      <c r="AC8" s="9"/>
-      <c r="AD8" s="9"/>
-      <c r="AE8" s="9"/>
-      <c r="AF8" s="9"/>
-      <c r="AG8" s="9"/>
-      <c r="AH8" s="9"/>
-      <c r="AI8" s="9"/>
-      <c r="AJ8" s="9"/>
-      <c r="AK8" s="9"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
+      <c r="P8" s="3"/>
+      <c r="Q8" s="3"/>
+      <c r="R8" s="3"/>
+      <c r="S8" s="3"/>
+      <c r="T8" s="3"/>
+      <c r="U8" s="3"/>
+      <c r="V8" s="3"/>
+      <c r="W8" s="3"/>
+      <c r="X8" s="3"/>
+      <c r="Y8" s="3"/>
+      <c r="Z8" s="3"/>
+      <c r="AA8" s="3"/>
+      <c r="AB8" s="3"/>
+      <c r="AC8" s="3"/>
+      <c r="AD8" s="3"/>
+      <c r="AE8" s="3"/>
+      <c r="AF8" s="3"/>
+      <c r="AG8" s="3"/>
+      <c r="AH8" s="3"/>
+      <c r="AI8" s="3"/>
+      <c r="AJ8" s="3"/>
+      <c r="AK8" s="3"/>
       <c r="AL8" s="1"/>
     </row>
     <row r="9" spans="1:38" ht="24" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="7" t="s">
         <v>3</v>
       </c>
       <c r="C9" s="2"/>
-      <c r="D9" s="13" t="s">
+      <c r="D9" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="9"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="14"/>
-      <c r="L9" s="14"/>
-      <c r="M9" s="14"/>
-      <c r="N9" s="14"/>
-      <c r="O9" s="14"/>
-      <c r="P9" s="14"/>
-      <c r="Q9" s="14"/>
-      <c r="R9" s="14"/>
-      <c r="S9" s="14"/>
-      <c r="T9" s="14"/>
-      <c r="U9" s="14"/>
-      <c r="V9" s="14"/>
-      <c r="W9" s="14"/>
-      <c r="X9" s="14"/>
-      <c r="Y9" s="14"/>
-      <c r="Z9" s="14"/>
-      <c r="AA9" s="14"/>
-      <c r="AB9" s="14"/>
-      <c r="AC9" s="14"/>
-      <c r="AD9" s="14"/>
-      <c r="AE9" s="14"/>
-      <c r="AF9" s="14"/>
-      <c r="AG9" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="AH9" s="16"/>
-      <c r="AI9" s="17"/>
-      <c r="AJ9" s="18" t="s">
+      <c r="E9" s="3"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
+      <c r="M9" s="8"/>
+      <c r="N9" s="8"/>
+      <c r="O9" s="8"/>
+      <c r="P9" s="8"/>
+      <c r="Q9" s="8"/>
+      <c r="R9" s="8"/>
+      <c r="S9" s="8"/>
+      <c r="T9" s="8"/>
+      <c r="U9" s="8"/>
+      <c r="V9" s="8"/>
+      <c r="W9" s="8"/>
+      <c r="X9" s="8"/>
+      <c r="Y9" s="8"/>
+      <c r="Z9" s="8"/>
+      <c r="AA9" s="8"/>
+      <c r="AB9" s="8"/>
+      <c r="AC9" s="8"/>
+      <c r="AD9" s="8"/>
+      <c r="AE9" s="8"/>
+      <c r="AF9" s="8"/>
+      <c r="AG9" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="AK9" s="18" t="s">
+      <c r="AH9" s="20"/>
+      <c r="AI9" s="21"/>
+      <c r="AJ9" s="9" t="s">
         <v>18</v>
+      </c>
+      <c r="AK9" s="9" t="s">
+        <v>17</v>
       </c>
       <c r="AL9" s="1"/>
     </row>
     <row r="10" spans="1:38" ht="24" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C10" s="2"/>
-      <c r="D10" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="E10" s="9"/>
-      <c r="F10" s="19" t="s">
+      <c r="D10" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" s="3"/>
+      <c r="F10" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="G10" s="20"/>
-      <c r="H10" s="20"/>
-      <c r="I10" s="20"/>
-      <c r="J10" s="20"/>
-      <c r="K10" s="20"/>
-      <c r="L10" s="20"/>
-      <c r="M10" s="21"/>
-      <c r="N10" s="19" t="s">
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="11"/>
+      <c r="M10" s="12"/>
+      <c r="N10" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="O10" s="20"/>
-      <c r="P10" s="20"/>
-      <c r="Q10" s="20"/>
-      <c r="R10" s="20"/>
-      <c r="S10" s="20"/>
-      <c r="T10" s="20"/>
-      <c r="U10" s="21"/>
-      <c r="V10" s="19" t="s">
+      <c r="O10" s="11"/>
+      <c r="P10" s="11"/>
+      <c r="Q10" s="11"/>
+      <c r="R10" s="11"/>
+      <c r="S10" s="11"/>
+      <c r="T10" s="11"/>
+      <c r="U10" s="12"/>
+      <c r="V10" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="W10" s="20"/>
-      <c r="X10" s="20"/>
-      <c r="Y10" s="20"/>
-      <c r="Z10" s="20"/>
-      <c r="AA10" s="20"/>
-      <c r="AB10" s="20"/>
-      <c r="AC10" s="21"/>
-      <c r="AD10" s="19" t="s">
+      <c r="W10" s="11"/>
+      <c r="X10" s="11"/>
+      <c r="Y10" s="11"/>
+      <c r="Z10" s="11"/>
+      <c r="AA10" s="11"/>
+      <c r="AB10" s="11"/>
+      <c r="AC10" s="12"/>
+      <c r="AD10" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="AE10" s="20"/>
-      <c r="AF10" s="20"/>
-      <c r="AG10" s="20"/>
-      <c r="AH10" s="20"/>
-      <c r="AI10" s="20"/>
-      <c r="AJ10" s="20"/>
-      <c r="AK10" s="21"/>
+      <c r="AE10" s="11"/>
+      <c r="AF10" s="11"/>
+      <c r="AG10" s="11"/>
+      <c r="AH10" s="11"/>
+      <c r="AI10" s="11"/>
+      <c r="AJ10" s="11"/>
+      <c r="AK10" s="12"/>
       <c r="AL10" s="1"/>
     </row>
     <row r="11" spans="1:38" ht="24" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C11" s="2"/>
-      <c r="D11" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="E11" s="9"/>
-      <c r="F11" s="19" t="s">
+      <c r="D11" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" s="3"/>
+      <c r="F11" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="G11" s="20"/>
-      <c r="H11" s="20"/>
-      <c r="I11" s="20"/>
-      <c r="J11" s="20"/>
-      <c r="K11" s="20"/>
-      <c r="L11" s="20"/>
-      <c r="M11" s="21"/>
-      <c r="N11" s="19" t="s">
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="11"/>
+      <c r="M11" s="12"/>
+      <c r="N11" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="O11" s="20"/>
-      <c r="P11" s="20"/>
-      <c r="Q11" s="20"/>
-      <c r="R11" s="20"/>
-      <c r="S11" s="20"/>
-      <c r="T11" s="20"/>
-      <c r="U11" s="21"/>
-      <c r="V11" s="19" t="s">
+      <c r="O11" s="11"/>
+      <c r="P11" s="11"/>
+      <c r="Q11" s="11"/>
+      <c r="R11" s="11"/>
+      <c r="S11" s="11"/>
+      <c r="T11" s="11"/>
+      <c r="U11" s="12"/>
+      <c r="V11" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="W11" s="20"/>
-      <c r="X11" s="20"/>
-      <c r="Y11" s="20"/>
-      <c r="Z11" s="20"/>
-      <c r="AA11" s="20"/>
-      <c r="AB11" s="20"/>
-      <c r="AC11" s="21"/>
-      <c r="AD11" s="19" t="s">
+      <c r="W11" s="11"/>
+      <c r="X11" s="11"/>
+      <c r="Y11" s="11"/>
+      <c r="Z11" s="11"/>
+      <c r="AA11" s="11"/>
+      <c r="AB11" s="11"/>
+      <c r="AC11" s="12"/>
+      <c r="AD11" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AE11" s="20"/>
-      <c r="AF11" s="20"/>
-      <c r="AG11" s="20"/>
-      <c r="AH11" s="20"/>
-      <c r="AI11" s="20"/>
-      <c r="AJ11" s="20"/>
-      <c r="AK11" s="21"/>
+      <c r="AE11" s="11"/>
+      <c r="AF11" s="11"/>
+      <c r="AG11" s="11"/>
+      <c r="AH11" s="11"/>
+      <c r="AI11" s="11"/>
+      <c r="AJ11" s="11"/>
+      <c r="AK11" s="12"/>
       <c r="AL11" s="1"/>
     </row>
     <row r="12" spans="1:38" ht="24" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C12" s="2"/>
-      <c r="D12" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="E12" s="9"/>
-      <c r="F12" s="19" t="s">
+      <c r="D12" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E12" s="3"/>
+      <c r="F12" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="G12" s="20"/>
-      <c r="H12" s="20"/>
-      <c r="I12" s="20"/>
-      <c r="J12" s="20"/>
-      <c r="K12" s="20"/>
-      <c r="L12" s="20"/>
-      <c r="M12" s="20"/>
-      <c r="N12" s="20"/>
-      <c r="O12" s="20"/>
-      <c r="P12" s="20"/>
-      <c r="Q12" s="20"/>
-      <c r="R12" s="20"/>
-      <c r="S12" s="20"/>
-      <c r="T12" s="20"/>
-      <c r="U12" s="20"/>
-      <c r="V12" s="20"/>
-      <c r="W12" s="20"/>
-      <c r="X12" s="20"/>
-      <c r="Y12" s="20"/>
-      <c r="Z12" s="20"/>
-      <c r="AA12" s="20"/>
-      <c r="AB12" s="20"/>
-      <c r="AC12" s="20"/>
-      <c r="AD12" s="20"/>
-      <c r="AE12" s="20"/>
-      <c r="AF12" s="20"/>
-      <c r="AG12" s="20"/>
-      <c r="AH12" s="20"/>
-      <c r="AI12" s="20"/>
-      <c r="AJ12" s="20"/>
-      <c r="AK12" s="21"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="11"/>
+      <c r="M12" s="11"/>
+      <c r="N12" s="11"/>
+      <c r="O12" s="11"/>
+      <c r="P12" s="11"/>
+      <c r="Q12" s="11"/>
+      <c r="R12" s="11"/>
+      <c r="S12" s="11"/>
+      <c r="T12" s="11"/>
+      <c r="U12" s="11"/>
+      <c r="V12" s="11"/>
+      <c r="W12" s="11"/>
+      <c r="X12" s="11"/>
+      <c r="Y12" s="11"/>
+      <c r="Z12" s="11"/>
+      <c r="AA12" s="11"/>
+      <c r="AB12" s="11"/>
+      <c r="AC12" s="11"/>
+      <c r="AD12" s="11"/>
+      <c r="AE12" s="11"/>
+      <c r="AF12" s="11"/>
+      <c r="AG12" s="11"/>
+      <c r="AH12" s="11"/>
+      <c r="AI12" s="11"/>
+      <c r="AJ12" s="11"/>
+      <c r="AK12" s="12"/>
       <c r="AL12" s="1"/>
     </row>
     <row r="13" spans="1:38" x14ac:dyDescent="0.2">

</xml_diff>